<commit_message>
finish intersection calculation when there must be one for everyone
</commit_message>
<xml_diff>
--- a/src/main/resources/t3.xlsx
+++ b/src/main/resources/t3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/finn/repo/time-scheduler/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8476C80E-B59A-3E45-BAE0-B9528BDDF62C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B001B3-ABF2-144F-A84F-6EB84D36AC36}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="460" windowWidth="50060" windowHeight="28340" activeTab="1" xr2:uid="{B79D25B7-5550-B540-A36A-E2C0BE443EC4}"/>
+    <workbookView xWindow="33680" yWindow="460" windowWidth="17200" windowHeight="28340" xr2:uid="{B79D25B7-5550-B540-A36A-E2C0BE443EC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -493,8 +493,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E86" sqref="E86"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2086,13 +2086,13 @@
       <c r="D74" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E74" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G74" t="s">
+      <c r="G74" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H74" t="s">
@@ -2112,13 +2112,13 @@
       <c r="D75" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E75" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G75" t="s">
+      <c r="G75" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H75" t="s">
@@ -2138,13 +2138,13 @@
       <c r="D76" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E76" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G76" t="s">
+      <c r="G76" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H76" t="s">
@@ -2164,13 +2164,13 @@
       <c r="D77" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E77" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G77" t="s">
+      <c r="G77" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H77" t="s">
@@ -2190,7 +2190,7 @@
       <c r="F78" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G78" t="s">
+      <c r="G78" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H78" t="s">
@@ -2210,7 +2210,7 @@
       <c r="F79" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G79" t="s">
+      <c r="G79" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H79" t="s">
@@ -2230,7 +2230,7 @@
       <c r="F80" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G80" t="s">
+      <c r="G80" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H80" t="s">
@@ -2250,7 +2250,7 @@
       <c r="F81" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G81" t="s">
+      <c r="G81" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H81" t="s">
@@ -2273,7 +2273,7 @@
       <c r="E82" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G82" t="s">
+      <c r="G82" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H82" t="s">
@@ -2296,7 +2296,7 @@
       <c r="E83" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G83" t="s">
+      <c r="G83" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H83" t="s">
@@ -2319,7 +2319,7 @@
       <c r="E84" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G84" t="s">
+      <c r="G84" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H84" t="s">
@@ -2342,7 +2342,7 @@
       <c r="E85" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G85" t="s">
+      <c r="G85" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H85" t="s">
@@ -2359,7 +2359,7 @@
       <c r="F86" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G86" t="s">
+      <c r="G86" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H86" t="s">
@@ -2376,7 +2376,7 @@
       <c r="F87" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G87" t="s">
+      <c r="G87" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H87" t="s">
@@ -2393,7 +2393,7 @@
       <c r="F88" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G88" t="s">
+      <c r="G88" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H88" t="s">
@@ -2410,7 +2410,7 @@
       <c r="F89" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G89" t="s">
+      <c r="G89" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H89" t="s">
@@ -2427,7 +2427,7 @@
       <c r="C90" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G90" t="s">
+      <c r="G90" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H90" t="s">
@@ -2444,7 +2444,7 @@
       <c r="C91" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G91" t="s">
+      <c r="G91" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H91" t="s">
@@ -2461,7 +2461,7 @@
       <c r="C92" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G92" t="s">
+      <c r="G92" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H92" t="s">
@@ -2478,7 +2478,7 @@
       <c r="C93" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G93" t="s">
+      <c r="G93" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H93" t="s">
@@ -2495,13 +2495,13 @@
       <c r="C94" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E94" t="s">
+      <c r="E94" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G94" t="s">
+      <c r="G94" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H94" t="s">
@@ -2518,13 +2518,13 @@
       <c r="C95" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E95" t="s">
+      <c r="E95" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G95" t="s">
+      <c r="G95" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H95" t="s">
@@ -2541,13 +2541,13 @@
       <c r="C96" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E96" t="s">
+      <c r="E96" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F96" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G96" t="s">
+      <c r="G96" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H96" t="s">
@@ -2564,13 +2564,13 @@
       <c r="C97" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E97" t="s">
+      <c r="E97" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F97" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G97" t="s">
+      <c r="G97" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H97" t="s">
@@ -2589,7 +2589,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>

</xml_diff>